<commit_message>
comparador de torque funcionando
</commit_message>
<xml_diff>
--- a/conversores.xlsx
+++ b/conversores.xlsx
@@ -421,7 +421,7 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -441,11 +441,11 @@
     </row>
     <row r="2" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
-        <v>42</v>
+        <v>103.6</v>
       </c>
       <c r="B2" s="5" t="n">
         <f aca="false">A2*0.102</f>
-        <v>4.284</v>
+        <v>10.5672</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -458,11 +458,11 @@
     </row>
     <row r="4" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
-        <v>42</v>
+        <v>103.6</v>
       </c>
       <c r="B4" s="7" t="n">
         <f aca="false">A4*0.7375621493</f>
-        <v>30.9776102706</v>
+        <v>76.41143866748</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -521,11 +521,11 @@
     </row>
     <row r="13" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="n">
-        <v>30.38</v>
+        <v>116</v>
       </c>
       <c r="B13" s="4" t="n">
         <f aca="false">A13*1.3558179483</f>
-        <v>41.189749269354</v>
+        <v>157.2748820028</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -538,17 +538,17 @@
     </row>
     <row r="15" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="n">
-        <v>30.38</v>
+        <v>116</v>
       </c>
       <c r="B15" s="5" t="n">
         <f aca="false">A15*0.1382549544</f>
-        <v>4.200185514672</v>
+        <v>16.0375747104</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>

</xml_diff>